<commit_message>
Clean test sheet made, and passing the test
</commit_message>
<xml_diff>
--- a/test_files/compress_missing_data_test/clean_sheet-compress-missing-data.xlsx
+++ b/test_files/compress_missing_data_test/clean_sheet-compress-missing-data.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="production_rates" sheetId="1" r:id="rId1"/>
+    <sheet name="degradation_rates" sheetId="2" r:id="rId2"/>
+    <sheet name="wt_log2_expression" sheetId="3" r:id="rId3"/>
+    <sheet name="dcin5_log2_expression" sheetId="4" r:id="rId4"/>
+    <sheet name="network" sheetId="5" r:id="rId5"/>
+    <sheet name="network_weights" sheetId="6" r:id="rId6"/>
+    <sheet name="optimization_parameters" sheetId="7" r:id="rId7"/>
+    <sheet name="threshold_b" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +25,100 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>production_rate</t>
+  </si>
+  <si>
+    <t>ACE2</t>
+  </si>
+  <si>
+    <t>AFT2</t>
+  </si>
+  <si>
+    <t>CIN5</t>
+  </si>
+  <si>
+    <t>FHL1</t>
+  </si>
+  <si>
+    <t>cols regulators/rows targets</t>
+  </si>
+  <si>
+    <t>cols regulators/row targets</t>
+  </si>
+  <si>
+    <t>optimization_parameter</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>kk_max</t>
+  </si>
+  <si>
+    <t>MaxIter</t>
+  </si>
+  <si>
+    <t>TolFun</t>
+  </si>
+  <si>
+    <t>MaxFunEval</t>
+  </si>
+  <si>
+    <t>TolX</t>
+  </si>
+  <si>
+    <t>production_function</t>
+  </si>
+  <si>
+    <t>L_curve</t>
+  </si>
+  <si>
+    <t>estimate_params</t>
+  </si>
+  <si>
+    <t>make_graphs</t>
+  </si>
+  <si>
+    <t>fix_P</t>
+  </si>
+  <si>
+    <t>fix_b</t>
+  </si>
+  <si>
+    <t>expression_timepoints</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>simulation_timepoints</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>dcin5</t>
+  </si>
+  <si>
+    <t>threshold_b</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +429,1037 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="4.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36D199C-5FF6-4580-AAA7-DF8075352B2C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="13.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5034CD7C-7AA5-40EF-8B26-9841D8460FBB}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0.4</v>
+      </c>
+      <c r="C1">
+        <v>0.4</v>
+      </c>
+      <c r="D1">
+        <v>0.4</v>
+      </c>
+      <c r="E1">
+        <v>0.8</v>
+      </c>
+      <c r="F1">
+        <v>0.8</v>
+      </c>
+      <c r="G1">
+        <v>0.8</v>
+      </c>
+      <c r="H1">
+        <v>1.2</v>
+      </c>
+      <c r="I1">
+        <v>1.2</v>
+      </c>
+      <c r="J1">
+        <v>1.2</v>
+      </c>
+      <c r="K1">
+        <v>1.6</v>
+      </c>
+      <c r="L1">
+        <v>1.6</v>
+      </c>
+      <c r="M1">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>111</v>
+      </c>
+      <c r="C2">
+        <v>112</v>
+      </c>
+      <c r="D2">
+        <v>113</v>
+      </c>
+      <c r="E2">
+        <v>211</v>
+      </c>
+      <c r="F2">
+        <v>212</v>
+      </c>
+      <c r="G2">
+        <v>213</v>
+      </c>
+      <c r="H2">
+        <v>311</v>
+      </c>
+      <c r="I2">
+        <v>312</v>
+      </c>
+      <c r="J2">
+        <v>313</v>
+      </c>
+      <c r="K2">
+        <v>411</v>
+      </c>
+      <c r="L2">
+        <v>412</v>
+      </c>
+      <c r="M2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>121</v>
+      </c>
+      <c r="C3">
+        <v>122</v>
+      </c>
+      <c r="D3">
+        <v>123</v>
+      </c>
+      <c r="E3">
+        <v>221</v>
+      </c>
+      <c r="F3">
+        <v>222</v>
+      </c>
+      <c r="G3">
+        <v>223</v>
+      </c>
+      <c r="H3">
+        <v>321</v>
+      </c>
+      <c r="I3">
+        <v>322</v>
+      </c>
+      <c r="J3">
+        <v>323</v>
+      </c>
+      <c r="K3">
+        <v>421</v>
+      </c>
+      <c r="L3">
+        <v>422</v>
+      </c>
+      <c r="M3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>131</v>
+      </c>
+      <c r="C4">
+        <v>132</v>
+      </c>
+      <c r="D4">
+        <v>133</v>
+      </c>
+      <c r="E4">
+        <v>231</v>
+      </c>
+      <c r="F4">
+        <v>232</v>
+      </c>
+      <c r="G4">
+        <v>233</v>
+      </c>
+      <c r="H4">
+        <v>331</v>
+      </c>
+      <c r="I4">
+        <v>332</v>
+      </c>
+      <c r="J4">
+        <v>333</v>
+      </c>
+      <c r="K4">
+        <v>431</v>
+      </c>
+      <c r="L4">
+        <v>432</v>
+      </c>
+      <c r="M4">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>141</v>
+      </c>
+      <c r="C5">
+        <v>142</v>
+      </c>
+      <c r="D5">
+        <v>143</v>
+      </c>
+      <c r="E5">
+        <v>241</v>
+      </c>
+      <c r="F5">
+        <v>242</v>
+      </c>
+      <c r="G5">
+        <v>243</v>
+      </c>
+      <c r="H5">
+        <v>341</v>
+      </c>
+      <c r="I5">
+        <v>342</v>
+      </c>
+      <c r="J5">
+        <v>343</v>
+      </c>
+      <c r="K5">
+        <v>441</v>
+      </c>
+      <c r="L5">
+        <v>442</v>
+      </c>
+      <c r="M5">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423A24F4-3C03-4912-B6A7-2CB682C9D6CD}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0.4</v>
+      </c>
+      <c r="C1">
+        <v>0.4</v>
+      </c>
+      <c r="D1">
+        <v>0.4</v>
+      </c>
+      <c r="E1">
+        <v>0.8</v>
+      </c>
+      <c r="F1">
+        <v>0.8</v>
+      </c>
+      <c r="G1">
+        <v>0.8</v>
+      </c>
+      <c r="H1">
+        <v>1.2</v>
+      </c>
+      <c r="I1">
+        <v>1.2</v>
+      </c>
+      <c r="J1">
+        <v>1.2</v>
+      </c>
+      <c r="K1">
+        <v>1.6</v>
+      </c>
+      <c r="L1">
+        <v>1.6</v>
+      </c>
+      <c r="M1">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>111</v>
+      </c>
+      <c r="C2">
+        <v>112</v>
+      </c>
+      <c r="D2">
+        <v>113</v>
+      </c>
+      <c r="E2">
+        <v>211</v>
+      </c>
+      <c r="F2">
+        <v>212</v>
+      </c>
+      <c r="G2">
+        <v>213</v>
+      </c>
+      <c r="H2">
+        <v>311</v>
+      </c>
+      <c r="I2">
+        <v>312</v>
+      </c>
+      <c r="J2">
+        <v>313</v>
+      </c>
+      <c r="K2">
+        <v>411</v>
+      </c>
+      <c r="L2">
+        <v>412</v>
+      </c>
+      <c r="M2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>121</v>
+      </c>
+      <c r="C3">
+        <v>122</v>
+      </c>
+      <c r="D3">
+        <v>123</v>
+      </c>
+      <c r="E3">
+        <v>221</v>
+      </c>
+      <c r="F3">
+        <v>222</v>
+      </c>
+      <c r="G3">
+        <v>223</v>
+      </c>
+      <c r="H3">
+        <v>321</v>
+      </c>
+      <c r="I3">
+        <v>322</v>
+      </c>
+      <c r="J3">
+        <v>323</v>
+      </c>
+      <c r="K3">
+        <v>421</v>
+      </c>
+      <c r="L3">
+        <v>422</v>
+      </c>
+      <c r="M3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>141</v>
+      </c>
+      <c r="C5">
+        <v>142</v>
+      </c>
+      <c r="D5">
+        <v>143</v>
+      </c>
+      <c r="E5">
+        <v>241</v>
+      </c>
+      <c r="F5">
+        <v>242</v>
+      </c>
+      <c r="G5">
+        <v>243</v>
+      </c>
+      <c r="H5">
+        <v>341</v>
+      </c>
+      <c r="I5">
+        <v>342</v>
+      </c>
+      <c r="J5">
+        <v>343</v>
+      </c>
+      <c r="K5">
+        <v>441</v>
+      </c>
+      <c r="L5">
+        <v>442</v>
+      </c>
+      <c r="M5">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115D046D-56C8-4058-BAC3-016CAF89EA88}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37800BEB-7495-4DC3-8876-0BECEFEEB167}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC888A0-A73F-49AB-BA98-BE8DD59226F5}">
+  <dimension ref="A1:V16"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>0.4</v>
+      </c>
+      <c r="C14">
+        <v>0.8</v>
+      </c>
+      <c r="D14">
+        <v>1.2</v>
+      </c>
+      <c r="E14">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0.1</v>
+      </c>
+      <c r="D16">
+        <v>0.2</v>
+      </c>
+      <c r="E16">
+        <v>0.3</v>
+      </c>
+      <c r="F16">
+        <v>0.4</v>
+      </c>
+      <c r="G16">
+        <v>0.5</v>
+      </c>
+      <c r="H16">
+        <v>0.6</v>
+      </c>
+      <c r="I16">
+        <v>0.7</v>
+      </c>
+      <c r="J16">
+        <v>0.8</v>
+      </c>
+      <c r="K16">
+        <v>0.9</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N16">
+        <v>1.2</v>
+      </c>
+      <c r="O16">
+        <v>1.3</v>
+      </c>
+      <c r="P16">
+        <v>1.4</v>
+      </c>
+      <c r="Q16">
+        <v>1.5</v>
+      </c>
+      <c r="R16">
+        <v>1.6</v>
+      </c>
+      <c r="S16">
+        <v>1.7</v>
+      </c>
+      <c r="T16">
+        <v>1.8</v>
+      </c>
+      <c r="U16">
+        <v>1.9</v>
+      </c>
+      <c r="V16">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE17433D-0F7C-481F-BEB2-7CDB92EE25AD}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>